<commit_message>
Module 2: News Sentiment Analysis project
</commit_message>
<xml_diff>
--- a/outputs/news_sentiment_report.xlsx
+++ b/outputs/news_sentiment_report.xlsx
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-0.85</v>
+        <v>-0.9</v>
       </c>
     </row>
     <row r="3">
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="5">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="6">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-0.75</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="7">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-0.9</v>
+        <v>-0.95</v>
       </c>
     </row>
     <row r="8">
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-0.75</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="9">
@@ -1074,7 +1074,7 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-0.6</v>
+        <v>-0.55</v>
       </c>
     </row>
     <row r="11">
@@ -1265,11 +1265,11 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>-0.95</v>
       </c>
     </row>
     <row r="14">
@@ -1393,11 +1393,11 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="16">
@@ -1456,11 +1456,11 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>-0.9</v>
       </c>
     </row>
     <row r="17">
@@ -1521,11 +1521,11 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="18">
@@ -1584,11 +1584,11 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>0</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="19">
@@ -1647,11 +1647,11 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="M19" t="n">
-        <v>0</v>
+        <v>-0.9</v>
       </c>
     </row>
     <row r="20">
@@ -1712,11 +1712,11 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>0</v>
+        <v>-0.9</v>
       </c>
     </row>
     <row r="21">
@@ -1773,11 +1773,11 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>0</v>
+        <v>-0.95</v>
       </c>
     </row>
     <row r="22">
@@ -1836,11 +1836,11 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="23">
@@ -1901,11 +1901,11 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="24">
@@ -1966,11 +1966,11 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="25">
@@ -2039,7 +2039,7 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-0.8</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="26">
@@ -2165,11 +2165,11 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>0.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -2230,11 +2230,11 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -2293,11 +2293,11 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -2354,11 +2354,11 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-0.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -2421,11 +2421,11 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>0.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -2484,11 +2484,11 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>0.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -2681,11 +2681,11 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>0.85</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="36">
@@ -2746,11 +2746,11 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="37">
@@ -2874,11 +2874,11 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="39">
@@ -2937,11 +2937,11 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>0</v>
+        <v>-0.95</v>
       </c>
     </row>
     <row r="40">
@@ -3004,11 +3004,11 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="41">
@@ -3067,11 +3067,11 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="42">
@@ -3130,11 +3130,11 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="43">
@@ -3191,11 +3191,11 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="44">
@@ -3256,11 +3256,11 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>0</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="45">
@@ -3319,11 +3319,11 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>0</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="46">
@@ -3451,7 +3451,7 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="48">
@@ -3512,7 +3512,7 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -3764,7 +3764,7 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="53">
@@ -3953,7 +3953,7 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="56">
@@ -4018,11 +4018,11 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -4396,11 +4396,11 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>0.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -4467,7 +4467,7 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="64">
@@ -4524,11 +4524,11 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-0.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -4589,11 +4589,11 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>negative</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -4650,11 +4650,11 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -4719,7 +4719,7 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="68">
@@ -4778,7 +4778,7 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-0.8</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="69">
@@ -4906,7 +4906,7 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="71">
@@ -4971,7 +4971,7 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-0.7</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="72">
@@ -5044,11 +5044,11 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>positive</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="73">
@@ -5111,11 +5111,11 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>0</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="74">
@@ -5174,11 +5174,11 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>0</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="75">
@@ -5239,11 +5239,11 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>0</v>
+        <v>-0.8</v>
       </c>
     </row>
     <row r="76">
@@ -5302,11 +5302,11 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>0</v>
+        <v>-0.95</v>
       </c>
     </row>
     <row r="77">
@@ -5812,11 +5812,11 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="85">
@@ -5875,11 +5875,11 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>negative</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>0</v>
+        <v>-0.95</v>
       </c>
     </row>
     <row r="86">
@@ -5946,7 +5946,7 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="87">
@@ -6072,7 +6072,7 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="89">
@@ -6194,11 +6194,11 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M90" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="91">
@@ -6263,7 +6263,7 @@
         </is>
       </c>
       <c r="M91" t="n">
-        <v>0.8</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="92">
@@ -6328,7 +6328,7 @@
         </is>
       </c>
       <c r="M92" t="n">
-        <v>-0.6</v>
+        <v>-0.35</v>
       </c>
     </row>
     <row r="93">
@@ -6391,7 +6391,7 @@
         </is>
       </c>
       <c r="M93" t="n">
-        <v>-0.8</v>
+        <v>-0.85</v>
       </c>
     </row>
     <row r="94">
@@ -6454,7 +6454,7 @@
         </is>
       </c>
       <c r="M94" t="n">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="95">
@@ -6637,11 +6637,11 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>positive</t>
         </is>
       </c>
       <c r="M97" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>